<commit_message>
Tukey's post-hoc on new metagenomic dataset
Currently running Tukey's post-hoc on the new metagenomic dataset. Still needs some rework before I'm done with this dataset.
</commit_message>
<xml_diff>
--- a/Statistical analyses/Compact letter displays/Litter chemistry/carboEster2, Precip, Tukey labels.xlsx
+++ b/Statistical analyses/Compact letter displays/Litter chemistry/carboEster2, Precip, Tukey labels.xlsx
@@ -22,16 +22,16 @@
     <t>labels</t>
   </si>
   <si>
+    <t>Reduced</t>
+  </si>
+  <si>
     <t>Ambient</t>
   </si>
   <si>
-    <t>Reduced</t>
+    <t>b</t>
   </si>
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
 </sst>
 </file>

</xml_diff>